<commit_message>
doc: create insert data file for SakilaDWH
</commit_message>
<xml_diff>
--- a/Analysis/Sakila_Pivot_Analysis.xlsx
+++ b/Analysis/Sakila_Pivot_Analysis.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Education\Uni\DataWarehouse\Final\Sakila-DataWarehouse\Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Education\Uni\DataWarehouse\Final\Sakila-DataWarehouse\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34CF8D6-741B-45EB-BF55-98A97DE557A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D58C092-B229-46FA-B063-4F27E995022E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{27116563-2158-4F54-A24E-7BA4B603F6CB}"/>
   </bookViews>
@@ -19,8 +19,8 @@
   <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId3"/>
-    <pivotCache cacheId="1" r:id="rId4"/>
-    <pivotCache cacheId="2" r:id="rId5"/>
+    <pivotCache cacheId="2" r:id="rId4"/>
+    <pivotCache cacheId="14" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -243,7 +243,127 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="53">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <sz val="14"/>
@@ -293,6 +413,9 @@
       <font>
         <sz val="14"/>
       </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <font>
@@ -569,126 +692,6 @@
         <sz val="14"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -703,1067 +706,6 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:pivotSource>
-    <c:name>[Sakila_Pivot_Analysis.xlsx]Expense-Rental!PivotTable1</c:name>
-    <c:fmtId val="3"/>
-  </c:pivotSource>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:pivotFmts>
-      <c:pivotFmt>
-        <c:idx val="0"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="1"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="2"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="3"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="4"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-    </c:pivotFmts>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Expense-Rental'!$C$3:$C$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Expense-Rental'!$B$5:$B$15</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>Brazil</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>China</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>India</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Indonesia</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Japan</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Mexico</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Philippines</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Russian Federation</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Turkey</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>United States</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Expense-Rental'!$C$5:$C$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-DEA0-4FCE-9A37-BB82F7B53096}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Expense-Rental'!$D$3:$D$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Expense-Rental'!$B$5:$B$15</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>Brazil</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>China</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>India</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Indonesia</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Japan</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Mexico</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Philippines</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Russian Federation</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Turkey</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>United States</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Expense-Rental'!$D$5:$D$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>109</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>111</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>63</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>70</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-DEA0-4FCE-9A37-BB82F7B53096}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Expense-Rental'!$E$3:$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Expense-Rental'!$B$5:$B$15</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>Brazil</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>China</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>India</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Indonesia</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Japan</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Mexico</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Philippines</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Russian Federation</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Turkey</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>United States</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Expense-Rental'!$E$5:$E$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>113</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>198</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>208</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>117</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>117</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>83</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>106</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>152</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-DEA0-4FCE-9A37-BB82F7B53096}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Expense-Rental'!$F$3:$F$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Expense-Rental'!$B$5:$B$15</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>Brazil</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>China</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>India</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Indonesia</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Japan</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Mexico</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Philippines</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Russian Federation</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Turkey</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>United States</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Expense-Rental'!$F$5:$F$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>319</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>594</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>651</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>139</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>334</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>320</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>232</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>308</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>172</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>376</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-DEA0-4FCE-9A37-BB82F7B53096}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Expense-Rental'!$G$3:$G$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>8</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Expense-Rental'!$B$5:$B$15</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>Brazil</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>China</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>India</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Indonesia</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Japan</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Mexico</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Philippines</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Russian Federation</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Turkey</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>United States</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Expense-Rental'!$G$5:$G$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>259</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>579</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>137</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>290</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>205</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>235</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>134</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>359</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-DEA0-4FCE-9A37-BB82F7B53096}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1743386832"/>
-        <c:axId val="1743386352"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1743386832"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1743386352"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1743386352"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1743386832"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-  <c:extLst>
-    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
-      <c14:pivotOptions>
-        <c14:dropZoneFilter val="1"/>
-        <c14:dropZoneCategories val="1"/>
-        <c14:dropZoneData val="1"/>
-        <c14:dropZoneSeries val="1"/>
-        <c14:dropZonesVisible val="1"/>
-      </c14:pivotOptions>
-    </c:ext>
-    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
-      <c16:pivotOptions16>
-        <c16:showExpandCollapseFieldButtons val="1"/>
-      </c16:pivotOptions16>
-    </c:ext>
-  </c:extLst>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2063,6 +1005,224 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -2231,7 +1391,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-236C-44F6-96F6-CE4D58092795}"/>
+              <c16:uniqueId val="{00000007-F303-4CD1-B3A4-DD6877686B74}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2323,7 +1483,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-236C-44F6-96F6-CE4D58092795}"/>
+              <c16:uniqueId val="{00000008-F303-4CD1-B3A4-DD6877686B74}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2415,7 +1575,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-236C-44F6-96F6-CE4D58092795}"/>
+              <c16:uniqueId val="{00000009-F303-4CD1-B3A4-DD6877686B74}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2507,7 +1667,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-236C-44F6-96F6-CE4D58092795}"/>
+              <c16:uniqueId val="{0000000A-F303-4CD1-B3A4-DD6877686B74}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2729,7 +1889,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -5380,6 +4540,1067 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[Sakila_Pivot_Analysis.xlsx]Expense-Rental!PivotTable1</c:name>
+    <c:fmtId val="19"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Expense-Rental'!$C$3:$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Expense-Rental'!$B$5:$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>China</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>India</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Indonesia</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Japan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Mexico</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Philippines</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Russian Federation</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Turkey</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>United States</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Expense-Rental'!$C$5:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2C09-4B18-AA0A-ECB49ABAFCD6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Expense-Rental'!$D$3:$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Expense-Rental'!$B$5:$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>China</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>India</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Indonesia</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Japan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Mexico</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Philippines</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Russian Federation</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Turkey</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>United States</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Expense-Rental'!$D$5:$D$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>70</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2C09-4B18-AA0A-ECB49ABAFCD6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Expense-Rental'!$E$3:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Expense-Rental'!$B$5:$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>China</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>India</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Indonesia</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Japan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Mexico</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Philippines</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Russian Federation</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Turkey</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>United States</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Expense-Rental'!$E$5:$E$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>152</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2C09-4B18-AA0A-ECB49ABAFCD6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Expense-Rental'!$F$3:$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Expense-Rental'!$B$5:$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>China</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>India</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Indonesia</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Japan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Mexico</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Philippines</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Russian Federation</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Turkey</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>United States</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Expense-Rental'!$F$5:$F$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>319</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>594</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>651</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>334</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>308</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>376</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-2C09-4B18-AA0A-ECB49ABAFCD6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Expense-Rental'!$G$3:$G$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Expense-Rental'!$B$5:$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>China</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>India</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Indonesia</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Japan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Mexico</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Philippines</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Russian Federation</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Turkey</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>United States</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Expense-Rental'!$G$5:$G$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>259</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>579</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>359</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-2C09-4B18-AA0A-ECB49ABAFCD6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="91457199"/>
+        <c:axId val="91467279"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="91457199"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="91467279"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="91467279"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="91457199"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -7377,7 +7598,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -7485,6 +7706,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -7495,6 +7721,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -7526,6 +7757,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -7880,7 +8114,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -7937,7 +8171,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -7989,9 +8223,11 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
@@ -8004,16 +8240,18 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -8039,9 +8277,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -8054,7 +8289,7 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -8097,22 +8332,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -8217,8 +8453,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -8350,19 +8586,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -8396,7 +8633,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -8453,7 +8690,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -8504,13 +8741,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -8521,19 +8751,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="25400">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -8571,7 +8794,7 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -8614,23 +8837,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -8735,8 +8957,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -8868,20 +9090,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -10457,51 +10678,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>314661</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>6051</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>1057835</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>26894</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10D53756-C307-5C5B-1462-4B550059190D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>300317</xdr:colOff>
+      <xdr:colOff>638764</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>8965</xdr:rowOff>
+      <xdr:rowOff>50529</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>80682</xdr:colOff>
+      <xdr:colOff>414180</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>170330</xdr:rowOff>
+      <xdr:rowOff>211894</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10520,7 +10705,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -10545,6 +10730,42 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DB586DA-3F3F-5C77-3A13-0A04D201AA87}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>640977</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>8964</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>968189</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AF7B078-C426-A898-7D6D-D87847323B3F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10825,7 +11046,156 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Nhân Đức" refreshedDate="45423.685659374998" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{8D893EC8-69A0-4E4C-957A-7D7036DF3DE9}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Nhân Đức" refreshedDate="45423.706621064812" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{54EF5DB8-DFD6-45AB-8DAC-CA6A043B626E}">
+  <cacheSource type="external" connectionId="6"/>
+  <cacheFields count="4">
+    <cacheField name="[Dim Staff].[Staff Key].[Staff Key]" caption="Staff Key" numFmtId="0" hierarchy="16" level="1">
+      <sharedItems count="2">
+        <s v="[Dim Staff].[Staff Key].&amp;[1]" c="1"/>
+        <s v="[Dim Staff].[Staff Key].&amp;[2]" c="2"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Rental Date].[Year].[Year]" caption="Year" numFmtId="0" hierarchy="30" level="1">
+      <sharedItems count="2">
+        <s v="[Rental Date].[Year].&amp;[2005]" c="2005"/>
+        <s v="[Rental Date].[Year].&amp;[2006]" c="2006"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Measures].[Amount]" caption="Amount" numFmtId="0" hierarchy="43" level="32767"/>
+    <cacheField name="[Rental Date].[Month Of Year].[Month Of Year]" caption="Month Of Year" numFmtId="0" hierarchy="28" level="1">
+      <sharedItems count="5">
+        <s v="[Rental Date].[Month Of Year].&amp;[2]" c="2"/>
+        <s v="[Rental Date].[Month Of Year].&amp;[5]" c="5"/>
+        <s v="[Rental Date].[Month Of Year].&amp;[6]" c="6"/>
+        <s v="[Rental Date].[Month Of Year].&amp;[7]" c="7"/>
+        <s v="[Rental Date].[Month Of Year].&amp;[8]" c="8"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <cacheHierarchies count="52">
+    <cacheHierarchy uniqueName="[Dim Actor].[Actor Key]" caption="Actor Key" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Dim Actor].[Actor Key].[All]" allUniqueName="[Dim Actor].[Actor Key].[All]" dimensionUniqueName="[Dim Actor]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Dim Address].[Address]" caption="Address" attribute="1" defaultMemberUniqueName="[Dim Address].[Address].[All]" allUniqueName="[Dim Address].[Address].[All]" dimensionUniqueName="[Dim Address]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Dim Address].[Address Key]" caption="Address Key" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Dim Address].[Address Key].[All]" allUniqueName="[Dim Address].[Address Key].[All]" dimensionUniqueName="[Dim Address]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Dim Address].[AddressHierarchy]" caption="AddressHierarchy" defaultMemberUniqueName="[Dim Address].[AddressHierarchy].[All]" allUniqueName="[Dim Address].[AddressHierarchy].[All]" dimensionUniqueName="[Dim Address]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Dim Address].[City]" caption="City" attribute="1" defaultMemberUniqueName="[Dim Address].[City].[All]" allUniqueName="[Dim Address].[City].[All]" dimensionUniqueName="[Dim Address]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Dim Address].[Country]" caption="Country" attribute="1" defaultMemberUniqueName="[Dim Address].[Country].[All]" allUniqueName="[Dim Address].[Country].[All]" dimensionUniqueName="[Dim Address]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Dim Address].[District]" caption="District" attribute="1" defaultMemberUniqueName="[Dim Address].[District].[All]" allUniqueName="[Dim Address].[District].[All]" dimensionUniqueName="[Dim Address]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Dim Customers].[Customer Key]" caption="Customer Key" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Dim Customers].[Customer Key].[All]" allUniqueName="[Dim Customers].[Customer Key].[All]" dimensionUniqueName="[Dim Customers]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Dim Inventory].[Category Name]" caption="Category Name" attribute="1" defaultMemberUniqueName="[Dim Inventory].[Category Name].[All]" allUniqueName="[Dim Inventory].[Category Name].[All]" dimensionUniqueName="[Dim Inventory]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Dim Inventory].[CategoryHierarchy]" caption="CategoryHierarchy" defaultMemberUniqueName="[Dim Inventory].[CategoryHierarchy].[All]" allUniqueName="[Dim Inventory].[CategoryHierarchy].[All]" dimensionUniqueName="[Dim Inventory]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Dim Inventory].[Inventory Key]" caption="Inventory Key" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Dim Inventory].[Inventory Key].[All]" allUniqueName="[Dim Inventory].[Inventory Key].[All]" dimensionUniqueName="[Dim Inventory]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Dim Inventory].[Language]" caption="Language" attribute="1" defaultMemberUniqueName="[Dim Inventory].[Language].[All]" allUniqueName="[Dim Inventory].[Language].[All]" dimensionUniqueName="[Dim Inventory]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Dim Inventory].[Rating]" caption="Rating" attribute="1" defaultMemberUniqueName="[Dim Inventory].[Rating].[All]" allUniqueName="[Dim Inventory].[Rating].[All]" dimensionUniqueName="[Dim Inventory]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Dim Inventory].[Release Year]" caption="Release Year" attribute="1" defaultMemberUniqueName="[Dim Inventory].[Release Year].[All]" allUniqueName="[Dim Inventory].[Release Year].[All]" dimensionUniqueName="[Dim Inventory]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Dim Inventory].[ReleaseYearHierarchy]" caption="ReleaseYearHierarchy" defaultMemberUniqueName="[Dim Inventory].[ReleaseYearHierarchy].[All]" allUniqueName="[Dim Inventory].[ReleaseYearHierarchy].[All]" dimensionUniqueName="[Dim Inventory]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Dim Rental].[Rental Key]" caption="Rental Key" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Dim Rental].[Rental Key].[All]" allUniqueName="[Dim Rental].[Rental Key].[All]" dimensionUniqueName="[Dim Rental]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Dim Staff].[Staff Key]" caption="Staff Key" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Dim Staff].[Staff Key].[All]" allUniqueName="[Dim Staff].[Staff Key].[All]" dimensionUniqueName="[Dim Staff]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="0"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Payment Date].[Date]" caption="Payment Date.Date" attribute="1" defaultMemberUniqueName="[Payment Date].[Date].[All]" allUniqueName="[Payment Date].[Date].[All]" dimensionUniqueName="[Payment Date]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Payment Date].[Date Key]" caption="Payment Date.Date Key" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Payment Date].[Date Key].[All]" allUniqueName="[Payment Date].[Date Key].[All]" dimensionUniqueName="[Payment Date]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Payment Date].[DateHierarchy]" caption="Payment Date.DateHierarchy" defaultMemberUniqueName="[Payment Date].[DateHierarchy].[All]" allUniqueName="[Payment Date].[DateHierarchy].[All]" dimensionUniqueName="[Payment Date]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Payment Date].[Day Of Week]" caption="Payment Date.Day Of Week" attribute="1" defaultMemberUniqueName="[Payment Date].[Day Of Week].[All]" allUniqueName="[Payment Date].[Day Of Week].[All]" dimensionUniqueName="[Payment Date]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Payment Date].[Month Of Year]" caption="Payment Date.Month Of Year" attribute="1" defaultMemberUniqueName="[Payment Date].[Month Of Year].[All]" allUniqueName="[Payment Date].[Month Of Year].[All]" dimensionUniqueName="[Payment Date]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Payment Date].[Quarter]" caption="Payment Date.Quarter" attribute="1" defaultMemberUniqueName="[Payment Date].[Quarter].[All]" allUniqueName="[Payment Date].[Quarter].[All]" dimensionUniqueName="[Payment Date]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Payment Date].[Year]" caption="Payment Date.Year" attribute="1" defaultMemberUniqueName="[Payment Date].[Year].[All]" allUniqueName="[Payment Date].[Year].[All]" dimensionUniqueName="[Payment Date]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Rental Date].[Date]" caption="Rental Date.Date" attribute="1" defaultMemberUniqueName="[Rental Date].[Date].[All]" allUniqueName="[Rental Date].[Date].[All]" dimensionUniqueName="[Rental Date]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Rental Date].[Date Key]" caption="Rental Date.Date Key" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Rental Date].[Date Key].[All]" allUniqueName="[Rental Date].[Date Key].[All]" dimensionUniqueName="[Rental Date]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Rental Date].[DateHierarchy]" caption="Rental Date.DateHierarchy" defaultMemberUniqueName="[Rental Date].[DateHierarchy].[All]" allUniqueName="[Rental Date].[DateHierarchy].[All]" dimensionUniqueName="[Rental Date]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Rental Date].[Day Of Week]" caption="Rental Date.Day Of Week" attribute="1" defaultMemberUniqueName="[Rental Date].[Day Of Week].[All]" allUniqueName="[Rental Date].[Day Of Week].[All]" dimensionUniqueName="[Rental Date]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Rental Date].[Month Of Year]" caption="Rental Date.Month Of Year" attribute="1" defaultMemberUniqueName="[Rental Date].[Month Of Year].[All]" allUniqueName="[Rental Date].[Month Of Year].[All]" dimensionUniqueName="[Rental Date]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="3"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Rental Date].[Quarter]" caption="Rental Date.Quarter" attribute="1" defaultMemberUniqueName="[Rental Date].[Quarter].[All]" allUniqueName="[Rental Date].[Quarter].[All]" dimensionUniqueName="[Rental Date]" displayFolder="" count="2" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Rental Date].[Year]" caption="Rental Date.Year" attribute="1" defaultMemberUniqueName="[Rental Date].[Year].[All]" allUniqueName="[Rental Date].[Year].[All]" dimensionUniqueName="[Rental Date]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="1"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Quantity]" caption="Quantity" measure="1" displayFolder="" measureGroup="Fact Rental Expense" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Expense]" caption="Expense" measure="1" displayFolder="" measureGroup="Fact Rental Expense" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Total Expense]" caption="Total Expense" measure="1" displayFolder="" measureGroup="Fact Rental Expense" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Fact Rental Expense Count]" caption="Fact Rental Expense Count" measure="1" displayFolder="" measureGroup="Fact Rental Expense" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Remaining]" caption="Remaining" measure="1" displayFolder="" measureGroup="Fact BP Film Inventory" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Total Rental Amount]" caption="Total Rental Amount" measure="1" displayFolder="" measureGroup="Fact BP Film Inventory" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Fact BP Film Inventory Count]" caption="Fact BP Film Inventory Count" measure="1" displayFolder="" measureGroup="Fact BP Film Inventory" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Rental Film]" caption="Rental Film" measure="1" displayFolder="" measureGroup="Fact BP Film Actor" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Actor Famous]" caption="Actor Famous" measure="1" displayFolder="" measureGroup="Fact BP Film Actor" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Actor Category]" caption="Actor Category" measure="1" displayFolder="" measureGroup="Fact BP Film Actor" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Fact BP Film Actor Count]" caption="Fact BP Film Actor Count" measure="1" displayFolder="" measureGroup="Fact BP Film Actor" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Store Id]" caption="Store Id" measure="1" displayFolder="" measureGroup="Fact B Performance" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Amount]" caption="Amount" measure="1" displayFolder="" measureGroup="Fact B Performance" count="0" oneField="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="2"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Quantity - Fact B Performance]" caption="Quantity - Fact B Performance" measure="1" displayFolder="" measureGroup="Fact B Performance" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Fact B Performance Count]" caption="Fact B Performance Count" measure="1" displayFolder="" measureGroup="Fact B Performance" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Rental Id]" caption="Rental Id" measure="1" displayFolder="" measureGroup="Fact BP Customer" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Amount - Fact BP Customer]" caption="Amount - Fact BP Customer" measure="1" displayFolder="" measureGroup="Fact BP Customer" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Recency]" caption="Recency" measure="1" displayFolder="" measureGroup="Fact BP Customer" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Frequency]" caption="Frequency" measure="1" displayFolder="" measureGroup="Fact BP Customer" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Monetary]" caption="Monetary" measure="1" displayFolder="" measureGroup="Fact BP Customer" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Fact BP Customer Count]" caption="Fact BP Customer Count" measure="1" displayFolder="" measureGroup="Fact BP Customer" count="0"/>
+  </cacheHierarchies>
+  <kpis count="0"/>
+  <dimensions count="9">
+    <dimension name="Dim Actor" uniqueName="[Dim Actor]" caption="Dim Actor"/>
+    <dimension name="Dim Address" uniqueName="[Dim Address]" caption="Dim Address"/>
+    <dimension name="Dim Customers" uniqueName="[Dim Customers]" caption="Dim Customers"/>
+    <dimension name="Dim Inventory" uniqueName="[Dim Inventory]" caption="Dim Inventory"/>
+    <dimension name="Dim Rental" uniqueName="[Dim Rental]" caption="Dim Rental"/>
+    <dimension name="Dim Staff" uniqueName="[Dim Staff]" caption="Dim Staff"/>
+    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
+    <dimension name="Payment Date" uniqueName="[Payment Date]" caption="Payment Date"/>
+    <dimension name="Rental Date" uniqueName="[Rental Date]" caption="Rental Date"/>
+  </dimensions>
+  <measureGroups count="5">
+    <measureGroup name="Fact B Performance" caption="Fact B Performance"/>
+    <measureGroup name="Fact BP Customer" caption="Fact BP Customer"/>
+    <measureGroup name="Fact BP Film Actor" caption="Fact BP Film Actor"/>
+    <measureGroup name="Fact BP Film Inventory" caption="Fact BP Film Inventory"/>
+    <measureGroup name="Fact Rental Expense" caption="Fact Rental Expense"/>
+  </measureGroups>
+  <maps count="20">
+    <map measureGroup="0" dimension="1"/>
+    <map measureGroup="0" dimension="4"/>
+    <map measureGroup="0" dimension="5"/>
+    <map measureGroup="0" dimension="8"/>
+    <map measureGroup="1" dimension="1"/>
+    <map measureGroup="1" dimension="2"/>
+    <map measureGroup="1" dimension="4"/>
+    <map measureGroup="1" dimension="7"/>
+    <map measureGroup="1" dimension="8"/>
+    <map measureGroup="2" dimension="0"/>
+    <map measureGroup="2" dimension="3"/>
+    <map measureGroup="2" dimension="4"/>
+    <map measureGroup="2" dimension="8"/>
+    <map measureGroup="3" dimension="3"/>
+    <map measureGroup="3" dimension="4"/>
+    <map measureGroup="3" dimension="8"/>
+    <map measureGroup="4" dimension="1"/>
+    <map measureGroup="4" dimension="2"/>
+    <map measureGroup="4" dimension="4"/>
+    <map measureGroup="4" dimension="8"/>
+  </maps>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Nhân Đức" refreshedDate="45426.919233680557" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{8D893EC8-69A0-4E4C-957A-7D7036DF3DE9}">
   <cacheSource type="external" connectionId="5"/>
   <cacheFields count="4">
     <cacheField name="[Dim Address].[Country].[Country]" caption="Country" numFmtId="0" hierarchy="5" level="1">
@@ -10986,157 +11356,8 @@
 </pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Nhân Đức" refreshedDate="45423.706621064812" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{54EF5DB8-DFD6-45AB-8DAC-CA6A043B626E}">
-  <cacheSource type="external" connectionId="6"/>
-  <cacheFields count="4">
-    <cacheField name="[Dim Staff].[Staff Key].[Staff Key]" caption="Staff Key" numFmtId="0" hierarchy="16" level="1">
-      <sharedItems count="2">
-        <s v="[Dim Staff].[Staff Key].&amp;[1]" c="1"/>
-        <s v="[Dim Staff].[Staff Key].&amp;[2]" c="2"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Rental Date].[Year].[Year]" caption="Year" numFmtId="0" hierarchy="30" level="1">
-      <sharedItems count="2">
-        <s v="[Rental Date].[Year].&amp;[2005]" c="2005"/>
-        <s v="[Rental Date].[Year].&amp;[2006]" c="2006"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Measures].[Amount]" caption="Amount" numFmtId="0" hierarchy="43" level="32767"/>
-    <cacheField name="[Rental Date].[Month Of Year].[Month Of Year]" caption="Month Of Year" numFmtId="0" hierarchy="28" level="1">
-      <sharedItems count="5">
-        <s v="[Rental Date].[Month Of Year].&amp;[2]" c="2"/>
-        <s v="[Rental Date].[Month Of Year].&amp;[5]" c="5"/>
-        <s v="[Rental Date].[Month Of Year].&amp;[6]" c="6"/>
-        <s v="[Rental Date].[Month Of Year].&amp;[7]" c="7"/>
-        <s v="[Rental Date].[Month Of Year].&amp;[8]" c="8"/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-  <cacheHierarchies count="52">
-    <cacheHierarchy uniqueName="[Dim Actor].[Actor Key]" caption="Actor Key" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Dim Actor].[Actor Key].[All]" allUniqueName="[Dim Actor].[Actor Key].[All]" dimensionUniqueName="[Dim Actor]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Dim Address].[Address]" caption="Address" attribute="1" defaultMemberUniqueName="[Dim Address].[Address].[All]" allUniqueName="[Dim Address].[Address].[All]" dimensionUniqueName="[Dim Address]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Dim Address].[Address Key]" caption="Address Key" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Dim Address].[Address Key].[All]" allUniqueName="[Dim Address].[Address Key].[All]" dimensionUniqueName="[Dim Address]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Dim Address].[AddressHierarchy]" caption="AddressHierarchy" defaultMemberUniqueName="[Dim Address].[AddressHierarchy].[All]" allUniqueName="[Dim Address].[AddressHierarchy].[All]" dimensionUniqueName="[Dim Address]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Dim Address].[City]" caption="City" attribute="1" defaultMemberUniqueName="[Dim Address].[City].[All]" allUniqueName="[Dim Address].[City].[All]" dimensionUniqueName="[Dim Address]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Dim Address].[Country]" caption="Country" attribute="1" defaultMemberUniqueName="[Dim Address].[Country].[All]" allUniqueName="[Dim Address].[Country].[All]" dimensionUniqueName="[Dim Address]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Dim Address].[District]" caption="District" attribute="1" defaultMemberUniqueName="[Dim Address].[District].[All]" allUniqueName="[Dim Address].[District].[All]" dimensionUniqueName="[Dim Address]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Dim Customers].[Customer Key]" caption="Customer Key" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Dim Customers].[Customer Key].[All]" allUniqueName="[Dim Customers].[Customer Key].[All]" dimensionUniqueName="[Dim Customers]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Dim Inventory].[Category Name]" caption="Category Name" attribute="1" defaultMemberUniqueName="[Dim Inventory].[Category Name].[All]" allUniqueName="[Dim Inventory].[Category Name].[All]" dimensionUniqueName="[Dim Inventory]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Dim Inventory].[CategoryHierarchy]" caption="CategoryHierarchy" defaultMemberUniqueName="[Dim Inventory].[CategoryHierarchy].[All]" allUniqueName="[Dim Inventory].[CategoryHierarchy].[All]" dimensionUniqueName="[Dim Inventory]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Dim Inventory].[Inventory Key]" caption="Inventory Key" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Dim Inventory].[Inventory Key].[All]" allUniqueName="[Dim Inventory].[Inventory Key].[All]" dimensionUniqueName="[Dim Inventory]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Dim Inventory].[Language]" caption="Language" attribute="1" defaultMemberUniqueName="[Dim Inventory].[Language].[All]" allUniqueName="[Dim Inventory].[Language].[All]" dimensionUniqueName="[Dim Inventory]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Dim Inventory].[Rating]" caption="Rating" attribute="1" defaultMemberUniqueName="[Dim Inventory].[Rating].[All]" allUniqueName="[Dim Inventory].[Rating].[All]" dimensionUniqueName="[Dim Inventory]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Dim Inventory].[Release Year]" caption="Release Year" attribute="1" defaultMemberUniqueName="[Dim Inventory].[Release Year].[All]" allUniqueName="[Dim Inventory].[Release Year].[All]" dimensionUniqueName="[Dim Inventory]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Dim Inventory].[ReleaseYearHierarchy]" caption="ReleaseYearHierarchy" defaultMemberUniqueName="[Dim Inventory].[ReleaseYearHierarchy].[All]" allUniqueName="[Dim Inventory].[ReleaseYearHierarchy].[All]" dimensionUniqueName="[Dim Inventory]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Dim Rental].[Rental Key]" caption="Rental Key" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Dim Rental].[Rental Key].[All]" allUniqueName="[Dim Rental].[Rental Key].[All]" dimensionUniqueName="[Dim Rental]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Dim Staff].[Staff Key]" caption="Staff Key" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Dim Staff].[Staff Key].[All]" allUniqueName="[Dim Staff].[Staff Key].[All]" dimensionUniqueName="[Dim Staff]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="0"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Payment Date].[Date]" caption="Payment Date.Date" attribute="1" defaultMemberUniqueName="[Payment Date].[Date].[All]" allUniqueName="[Payment Date].[Date].[All]" dimensionUniqueName="[Payment Date]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Payment Date].[Date Key]" caption="Payment Date.Date Key" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Payment Date].[Date Key].[All]" allUniqueName="[Payment Date].[Date Key].[All]" dimensionUniqueName="[Payment Date]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Payment Date].[DateHierarchy]" caption="Payment Date.DateHierarchy" defaultMemberUniqueName="[Payment Date].[DateHierarchy].[All]" allUniqueName="[Payment Date].[DateHierarchy].[All]" dimensionUniqueName="[Payment Date]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Payment Date].[Day Of Week]" caption="Payment Date.Day Of Week" attribute="1" defaultMemberUniqueName="[Payment Date].[Day Of Week].[All]" allUniqueName="[Payment Date].[Day Of Week].[All]" dimensionUniqueName="[Payment Date]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Payment Date].[Month Of Year]" caption="Payment Date.Month Of Year" attribute="1" defaultMemberUniqueName="[Payment Date].[Month Of Year].[All]" allUniqueName="[Payment Date].[Month Of Year].[All]" dimensionUniqueName="[Payment Date]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Payment Date].[Quarter]" caption="Payment Date.Quarter" attribute="1" defaultMemberUniqueName="[Payment Date].[Quarter].[All]" allUniqueName="[Payment Date].[Quarter].[All]" dimensionUniqueName="[Payment Date]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Payment Date].[Year]" caption="Payment Date.Year" attribute="1" defaultMemberUniqueName="[Payment Date].[Year].[All]" allUniqueName="[Payment Date].[Year].[All]" dimensionUniqueName="[Payment Date]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Rental Date].[Date]" caption="Rental Date.Date" attribute="1" defaultMemberUniqueName="[Rental Date].[Date].[All]" allUniqueName="[Rental Date].[Date].[All]" dimensionUniqueName="[Rental Date]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Rental Date].[Date Key]" caption="Rental Date.Date Key" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Rental Date].[Date Key].[All]" allUniqueName="[Rental Date].[Date Key].[All]" dimensionUniqueName="[Rental Date]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Rental Date].[DateHierarchy]" caption="Rental Date.DateHierarchy" defaultMemberUniqueName="[Rental Date].[DateHierarchy].[All]" allUniqueName="[Rental Date].[DateHierarchy].[All]" dimensionUniqueName="[Rental Date]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Rental Date].[Day Of Week]" caption="Rental Date.Day Of Week" attribute="1" defaultMemberUniqueName="[Rental Date].[Day Of Week].[All]" allUniqueName="[Rental Date].[Day Of Week].[All]" dimensionUniqueName="[Rental Date]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Rental Date].[Month Of Year]" caption="Rental Date.Month Of Year" attribute="1" defaultMemberUniqueName="[Rental Date].[Month Of Year].[All]" allUniqueName="[Rental Date].[Month Of Year].[All]" dimensionUniqueName="[Rental Date]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="3"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Rental Date].[Quarter]" caption="Rental Date.Quarter" attribute="1" defaultMemberUniqueName="[Rental Date].[Quarter].[All]" allUniqueName="[Rental Date].[Quarter].[All]" dimensionUniqueName="[Rental Date]" displayFolder="" count="2" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Rental Date].[Year]" caption="Rental Date.Year" attribute="1" defaultMemberUniqueName="[Rental Date].[Year].[All]" allUniqueName="[Rental Date].[Year].[All]" dimensionUniqueName="[Rental Date]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="1"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Measures].[Quantity]" caption="Quantity" measure="1" displayFolder="" measureGroup="Fact Rental Expense" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Expense]" caption="Expense" measure="1" displayFolder="" measureGroup="Fact Rental Expense" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Total Expense]" caption="Total Expense" measure="1" displayFolder="" measureGroup="Fact Rental Expense" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Fact Rental Expense Count]" caption="Fact Rental Expense Count" measure="1" displayFolder="" measureGroup="Fact Rental Expense" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Remaining]" caption="Remaining" measure="1" displayFolder="" measureGroup="Fact BP Film Inventory" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Total Rental Amount]" caption="Total Rental Amount" measure="1" displayFolder="" measureGroup="Fact BP Film Inventory" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Fact BP Film Inventory Count]" caption="Fact BP Film Inventory Count" measure="1" displayFolder="" measureGroup="Fact BP Film Inventory" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Rental Film]" caption="Rental Film" measure="1" displayFolder="" measureGroup="Fact BP Film Actor" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Actor Famous]" caption="Actor Famous" measure="1" displayFolder="" measureGroup="Fact BP Film Actor" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Actor Category]" caption="Actor Category" measure="1" displayFolder="" measureGroup="Fact BP Film Actor" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Fact BP Film Actor Count]" caption="Fact BP Film Actor Count" measure="1" displayFolder="" measureGroup="Fact BP Film Actor" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Store Id]" caption="Store Id" measure="1" displayFolder="" measureGroup="Fact B Performance" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Amount]" caption="Amount" measure="1" displayFolder="" measureGroup="Fact B Performance" count="0" oneField="1">
-      <fieldsUsage count="1">
-        <fieldUsage x="2"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Measures].[Quantity - Fact B Performance]" caption="Quantity - Fact B Performance" measure="1" displayFolder="" measureGroup="Fact B Performance" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Fact B Performance Count]" caption="Fact B Performance Count" measure="1" displayFolder="" measureGroup="Fact B Performance" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Rental Id]" caption="Rental Id" measure="1" displayFolder="" measureGroup="Fact BP Customer" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Amount - Fact BP Customer]" caption="Amount - Fact BP Customer" measure="1" displayFolder="" measureGroup="Fact BP Customer" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Recency]" caption="Recency" measure="1" displayFolder="" measureGroup="Fact BP Customer" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Frequency]" caption="Frequency" measure="1" displayFolder="" measureGroup="Fact BP Customer" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Monetary]" caption="Monetary" measure="1" displayFolder="" measureGroup="Fact BP Customer" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Fact BP Customer Count]" caption="Fact BP Customer Count" measure="1" displayFolder="" measureGroup="Fact BP Customer" count="0"/>
-  </cacheHierarchies>
-  <kpis count="0"/>
-  <dimensions count="9">
-    <dimension name="Dim Actor" uniqueName="[Dim Actor]" caption="Dim Actor"/>
-    <dimension name="Dim Address" uniqueName="[Dim Address]" caption="Dim Address"/>
-    <dimension name="Dim Customers" uniqueName="[Dim Customers]" caption="Dim Customers"/>
-    <dimension name="Dim Inventory" uniqueName="[Dim Inventory]" caption="Dim Inventory"/>
-    <dimension name="Dim Rental" uniqueName="[Dim Rental]" caption="Dim Rental"/>
-    <dimension name="Dim Staff" uniqueName="[Dim Staff]" caption="Dim Staff"/>
-    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
-    <dimension name="Payment Date" uniqueName="[Payment Date]" caption="Payment Date"/>
-    <dimension name="Rental Date" uniqueName="[Rental Date]" caption="Rental Date"/>
-  </dimensions>
-  <measureGroups count="5">
-    <measureGroup name="Fact B Performance" caption="Fact B Performance"/>
-    <measureGroup name="Fact BP Customer" caption="Fact BP Customer"/>
-    <measureGroup name="Fact BP Film Actor" caption="Fact BP Film Actor"/>
-    <measureGroup name="Fact BP Film Inventory" caption="Fact BP Film Inventory"/>
-    <measureGroup name="Fact Rental Expense" caption="Fact Rental Expense"/>
-  </measureGroups>
-  <maps count="20">
-    <map measureGroup="0" dimension="1"/>
-    <map measureGroup="0" dimension="4"/>
-    <map measureGroup="0" dimension="5"/>
-    <map measureGroup="0" dimension="8"/>
-    <map measureGroup="1" dimension="1"/>
-    <map measureGroup="1" dimension="2"/>
-    <map measureGroup="1" dimension="4"/>
-    <map measureGroup="1" dimension="7"/>
-    <map measureGroup="1" dimension="8"/>
-    <map measureGroup="2" dimension="0"/>
-    <map measureGroup="2" dimension="3"/>
-    <map measureGroup="2" dimension="4"/>
-    <map measureGroup="2" dimension="8"/>
-    <map measureGroup="3" dimension="3"/>
-    <map measureGroup="3" dimension="4"/>
-    <map measureGroup="3" dimension="8"/>
-    <map measureGroup="4" dimension="1"/>
-    <map measureGroup="4" dimension="2"/>
-    <map measureGroup="4" dimension="4"/>
-    <map measureGroup="4" dimension="8"/>
-  </maps>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{98D678E2-EE3F-450C-826A-A4504FBF4941}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{98D678E2-EE3F-450C-826A-A4504FBF4941}" name="PivotTable2" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" fieldListSortAscending="1">
   <location ref="B24:H33" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField allDrilled="1" subtotalTop="0" showAll="0" measureFilter="1" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
@@ -11230,51 +11451,304 @@
   <dataFields count="1">
     <dataField fld="3" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="11">
-    <format dxfId="39">
+  <formats count="12">
+    <format dxfId="52">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="38">
+    <format dxfId="51">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="37">
+    <format dxfId="50">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="36">
+    <format dxfId="49">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="35">
+    <format dxfId="48">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="34">
+    <format dxfId="47">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="33">
+    <format dxfId="46">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="32">
+    <format dxfId="45">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="31">
+    <format dxfId="44">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="30">
+    <format dxfId="43">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="29">
+    <format dxfId="42">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
+    <format dxfId="22">
+      <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
   </formats>
-  <conditionalFormats count="13">
-    <conditionalFormat type="all" priority="1">
+  <conditionalFormats count="14">
+    <conditionalFormat priority="14">
+      <pivotAreas count="1">
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="7">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat type="all" priority="13">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="7">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat type="all" priority="12">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="7">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat type="all" priority="11">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="1" selected="0">
+              <x v="2"/>
+            </reference>
+            <reference field="2" count="7">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat type="all" priority="10">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="1" selected="0">
+              <x v="2"/>
+            </reference>
+            <reference field="2" count="7">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat type="all" priority="9">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="7">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat type="all" priority="8">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="1" selected="0">
+              <x v="2"/>
+            </reference>
+            <reference field="2" count="7">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat type="all" priority="7">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="2" count="7">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat type="all" priority="6">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="2" count="7">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat type="all" priority="5">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="1" selected="0">
+              <x v="4"/>
+            </reference>
+            <reference field="2" count="7">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat type="all" priority="4">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="1" selected="0">
+              <x v="4"/>
+            </reference>
+            <reference field="2" count="7">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat type="all" priority="3">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -11320,258 +11794,26 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat type="all" priority="3">
+    <conditionalFormat priority="1">
       <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
+        <pivotArea type="data" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
             <reference field="4294967294" count="1" selected="0">
               <x v="0"/>
             </reference>
-            <reference field="1" count="1" selected="0">
-              <x v="4"/>
-            </reference>
-            <reference field="2" count="7">
+            <reference field="1" count="5" selected="0">
               <x v="0"/>
               <x v="1"/>
               <x v="2"/>
               <x v="3"/>
               <x v="4"/>
-              <x v="5"/>
-              <x v="6"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat type="all" priority="4">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="1" selected="0">
-              <x v="4"/>
-            </reference>
-            <reference field="2" count="7">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-              <x v="6"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat type="all" priority="5">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="1" selected="0">
-              <x v="3"/>
-            </reference>
-            <reference field="2" count="7">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-              <x v="6"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat type="all" priority="6">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="1" selected="0">
-              <x v="3"/>
-            </reference>
-            <reference field="2" count="7">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-              <x v="6"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat type="all" priority="7">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="1" selected="0">
-              <x v="2"/>
-            </reference>
-            <reference field="2" count="7">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-              <x v="6"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat type="all" priority="8">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="1" selected="0">
-              <x v="1"/>
-            </reference>
-            <reference field="2" count="7">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-              <x v="6"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat type="all" priority="9">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="1" selected="0">
-              <x v="2"/>
-            </reference>
-            <reference field="2" count="7">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-              <x v="6"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat type="all" priority="10">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="1" selected="0">
-              <x v="2"/>
-            </reference>
-            <reference field="2" count="7">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-              <x v="6"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat type="all" priority="11">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="1" selected="0">
-              <x v="1"/>
-            </reference>
-            <reference field="2" count="7">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-              <x v="6"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat type="all" priority="12">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="1" selected="0">
-              <x v="1"/>
-            </reference>
-            <reference field="2" count="7">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-              <x v="6"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="13">
-      <pivotAreas count="1">
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="7">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-              <x v="6"/>
             </reference>
           </references>
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
   </conditionalFormats>
-  <chartFormats count="5">
+  <chartFormats count="12">
     <chartFormat chart="7" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
@@ -11628,6 +11870,87 @@
           </reference>
           <reference field="1" count="1" selected="0">
             <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="11" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="6"/>
           </reference>
         </references>
       </pivotArea>
@@ -11715,7 +12038,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9E0BCB3F-52BE-43BD-BD55-F1668490D9F8}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="18" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9E0BCB3F-52BE-43BD-BD55-F1668490D9F8}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="20" fieldListSortAscending="1">
   <location ref="B3:H15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -11808,47 +12131,47 @@
     <dataField fld="0" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="10">
-    <format dxfId="0">
+    <format dxfId="12">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="1">
+    <format dxfId="13">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="2">
+    <format dxfId="14">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="3">
+    <format dxfId="15">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="4">
+    <format dxfId="16">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="5">
+    <format dxfId="17">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="6">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="19">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="8">
+    <format dxfId="20">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="21">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
   <conditionalFormats count="1">
-    <conditionalFormat priority="25">
+    <conditionalFormat priority="26">
       <pivotAreas count="1">
         <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="2">
@@ -11873,66 +12196,6 @@
     </conditionalFormat>
   </conditionalFormats>
   <chartFormats count="60">
-    <chartFormat chart="3" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="3" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="4" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
     <chartFormat chart="17" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
@@ -12736,6 +12999,66 @@
           </reference>
           <reference field="1" count="1" selected="0">
             <x v="9"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="19" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="19" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="19" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="19" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="19" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
           </reference>
           <reference field="2" count="1" selected="0">
             <x v="4"/>
@@ -12818,7 +13141,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1">
         <x14:conditionalFormats count="5">
-          <x14:conditionalFormat priority="20" id="{B63F468B-07FD-4255-908B-DD90BC519718}">
+          <x14:conditionalFormat priority="25" id="{15745E97-9939-4517-8A04-29D4F9D687C5}">
             <x14:pivotAreas count="1">
               <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
                 <references count="3">
@@ -12838,13 +13161,65 @@
                     <x v="9"/>
                   </reference>
                   <reference field="2" count="1" selected="0">
-                    <x v="4"/>
+                    <x v="0"/>
                   </reference>
                 </references>
               </pivotArea>
             </x14:pivotAreas>
           </x14:conditionalFormat>
-          <x14:conditionalFormat priority="21" id="{1D7458E5-6B23-4A90-A3E6-1C9739B17A2D}">
+          <x14:conditionalFormat priority="24" id="{04114CB4-E864-4CD6-BA10-54494549D5F4}">
+            <x14:pivotAreas count="1">
+              <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+                <references count="3">
+                  <reference field="4294967294" count="1" selected="0">
+                    <x v="0"/>
+                  </reference>
+                  <reference field="1" count="10">
+                    <x v="0"/>
+                    <x v="1"/>
+                    <x v="2"/>
+                    <x v="3"/>
+                    <x v="4"/>
+                    <x v="5"/>
+                    <x v="6"/>
+                    <x v="7"/>
+                    <x v="8"/>
+                    <x v="9"/>
+                  </reference>
+                  <reference field="2" count="1" selected="0">
+                    <x v="1"/>
+                  </reference>
+                </references>
+              </pivotArea>
+            </x14:pivotAreas>
+          </x14:conditionalFormat>
+          <x14:conditionalFormat priority="23" id="{16DD4843-82D4-4567-86B3-F15723CB8520}">
+            <x14:pivotAreas count="1">
+              <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+                <references count="3">
+                  <reference field="4294967294" count="1" selected="0">
+                    <x v="0"/>
+                  </reference>
+                  <reference field="1" count="10">
+                    <x v="0"/>
+                    <x v="1"/>
+                    <x v="2"/>
+                    <x v="3"/>
+                    <x v="4"/>
+                    <x v="5"/>
+                    <x v="6"/>
+                    <x v="7"/>
+                    <x v="8"/>
+                    <x v="9"/>
+                  </reference>
+                  <reference field="2" count="1" selected="0">
+                    <x v="2"/>
+                  </reference>
+                </references>
+              </pivotArea>
+            </x14:pivotAreas>
+          </x14:conditionalFormat>
+          <x14:conditionalFormat priority="22" id="{1D7458E5-6B23-4A90-A3E6-1C9739B17A2D}">
             <x14:pivotAreas count="1">
               <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
                 <references count="3">
@@ -12870,7 +13245,7 @@
               </pivotArea>
             </x14:pivotAreas>
           </x14:conditionalFormat>
-          <x14:conditionalFormat priority="22" id="{16DD4843-82D4-4567-86B3-F15723CB8520}">
+          <x14:conditionalFormat priority="21" id="{B63F468B-07FD-4255-908B-DD90BC519718}">
             <x14:pivotAreas count="1">
               <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
                 <references count="3">
@@ -12890,59 +13265,7 @@
                     <x v="9"/>
                   </reference>
                   <reference field="2" count="1" selected="0">
-                    <x v="2"/>
-                  </reference>
-                </references>
-              </pivotArea>
-            </x14:pivotAreas>
-          </x14:conditionalFormat>
-          <x14:conditionalFormat priority="23" id="{04114CB4-E864-4CD6-BA10-54494549D5F4}">
-            <x14:pivotAreas count="1">
-              <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-                <references count="3">
-                  <reference field="4294967294" count="1" selected="0">
-                    <x v="0"/>
-                  </reference>
-                  <reference field="1" count="10">
-                    <x v="0"/>
-                    <x v="1"/>
-                    <x v="2"/>
-                    <x v="3"/>
                     <x v="4"/>
-                    <x v="5"/>
-                    <x v="6"/>
-                    <x v="7"/>
-                    <x v="8"/>
-                    <x v="9"/>
-                  </reference>
-                  <reference field="2" count="1" selected="0">
-                    <x v="1"/>
-                  </reference>
-                </references>
-              </pivotArea>
-            </x14:pivotAreas>
-          </x14:conditionalFormat>
-          <x14:conditionalFormat priority="24" id="{15745E97-9939-4517-8A04-29D4F9D687C5}">
-            <x14:pivotAreas count="1">
-              <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-                <references count="3">
-                  <reference field="4294967294" count="1" selected="0">
-                    <x v="0"/>
-                  </reference>
-                  <reference field="1" count="10">
-                    <x v="0"/>
-                    <x v="1"/>
-                    <x v="2"/>
-                    <x v="3"/>
-                    <x v="4"/>
-                    <x v="5"/>
-                    <x v="6"/>
-                    <x v="7"/>
-                    <x v="8"/>
-                    <x v="9"/>
-                  </reference>
-                  <reference field="2" count="1" selected="0">
-                    <x v="0"/>
                   </reference>
                 </references>
               </pivotArea>
@@ -13048,7 +13371,7 @@
     <dataField fld="2" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="8">
-    <format dxfId="28">
+    <format dxfId="41">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -13057,10 +13380,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="27">
+    <format dxfId="40">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="26">
+    <format dxfId="39">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
@@ -13072,7 +13395,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="25">
+    <format dxfId="38">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -13085,7 +13408,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="24">
+    <format dxfId="37">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
@@ -13097,7 +13420,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="23">
+    <format dxfId="36">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -13110,73 +13433,15 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="22">
+    <format dxfId="35">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="21">
+    <format dxfId="34">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
   </formats>
   <conditionalFormats count="4">
-    <conditionalFormat priority="7">
-      <pivotAreas count="4">
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="0" count="1">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="0" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="3" count="5">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="0" count="1">
-              <x v="1"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="0" count="1" selected="0">
-              <x v="1"/>
-            </reference>
-            <reference field="3" count="5">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="8">
+    <conditionalFormat priority="10">
       <pivotAreas count="4">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -13316,7 +13581,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="10">
+    <conditionalFormat priority="8">
       <pivotAreas count="4">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -13374,6 +13639,64 @@
             </reference>
             <reference field="1" count="1" selected="0">
               <x v="0"/>
+            </reference>
+            <reference field="3" count="5">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="7">
+      <pivotAreas count="4">
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="0" count="1">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="0" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="3" count="5">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="0" count="1">
+              <x v="1"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="0" count="1" selected="0">
+              <x v="1"/>
             </reference>
             <reference field="3" count="5">
               <x v="0"/>
@@ -13487,13 +13810,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{54635CDB-36B2-4D32-BC3D-3B59FD62E736}" name="Table4" displayName="Table4" ref="B27:E33" totalsRowCount="1" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{54635CDB-36B2-4D32-BC3D-3B59FD62E736}" name="Table4" displayName="Table4" ref="B27:E33" totalsRowCount="1" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32">
   <autoFilter ref="B27:E32" xr:uid="{54635CDB-36B2-4D32-BC3D-3B59FD62E736}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8500DC3C-C701-403A-9257-70D96E5535CE}" name="Month" totalsRowLabel="Total" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{776E815B-7758-40E2-A54A-B26203A1370B}" name="1" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{A3588CCD-68F4-439E-9566-A72EA12597C6}" name="2" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{2B539642-9B3B-483C-9EF7-9C00B333C0E7}" name="Quantity" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{8500DC3C-C701-403A-9257-70D96E5535CE}" name="Month" totalsRowLabel="Total" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{776E815B-7758-40E2-A54A-B26203A1370B}" name="1" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{A3588CCD-68F4-439E-9566-A72EA12597C6}" name="2" totalsRowFunction="sum" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{2B539642-9B3B-483C-9EF7-9C00B333C0E7}" name="Quantity" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13818,21 +14141,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EBBA9D3-0048-4D30-8DE7-49F83EE6D522}">
   <dimension ref="A2:I151"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="X27" sqref="X27:Y27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" customWidth="1"/>
-    <col min="6" max="6" width="17.109375" customWidth="1"/>
-    <col min="7" max="7" width="16.77734375" customWidth="1"/>
-    <col min="8" max="8" width="17.109375" customWidth="1"/>
-    <col min="9" max="9" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="18" width="7" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.5546875" bestFit="1" customWidth="1"/>
@@ -14612,10 +14935,29 @@
     <row r="40" spans="2:8" ht="18" x14ac:dyDescent="0.35"/>
     <row r="41" spans="2:8" ht="18" x14ac:dyDescent="0.35"/>
     <row r="42" spans="2:8" ht="18" x14ac:dyDescent="0.35"/>
+    <row r="43" spans="2:8" ht="18" x14ac:dyDescent="0.35"/>
+    <row r="44" spans="2:8" ht="18" x14ac:dyDescent="0.35"/>
+    <row r="45" spans="2:8" ht="18" x14ac:dyDescent="0.35"/>
+    <row r="46" spans="2:8" ht="18" x14ac:dyDescent="0.35"/>
+    <row r="47" spans="2:8" ht="18" x14ac:dyDescent="0.35"/>
+    <row r="48" spans="2:8" ht="18" x14ac:dyDescent="0.35"/>
+    <row r="49" ht="18" x14ac:dyDescent="0.35"/>
+    <row r="50" ht="18" x14ac:dyDescent="0.35"/>
+    <row r="51" ht="18" x14ac:dyDescent="0.35"/>
+    <row r="52" ht="18" x14ac:dyDescent="0.35"/>
+    <row r="53" ht="18" x14ac:dyDescent="0.35"/>
+    <row r="54" ht="18" x14ac:dyDescent="0.35"/>
+    <row r="55" ht="18" x14ac:dyDescent="0.35"/>
+    <row r="56" ht="18" x14ac:dyDescent="0.35"/>
+    <row r="57" ht="18" x14ac:dyDescent="0.35"/>
+    <row r="58" ht="18" x14ac:dyDescent="0.35"/>
+    <row r="59" ht="18" x14ac:dyDescent="0.35"/>
+    <row r="60" ht="18" x14ac:dyDescent="0.35"/>
+    <row r="61" ht="18" x14ac:dyDescent="0.35"/>
     <row r="151" ht="24.6" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <conditionalFormatting sqref="C2">
-    <cfRule type="dataBar" priority="42">
+    <cfRule type="dataBar" priority="43">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -14629,7 +14971,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="H5:H14">
-    <cfRule type="colorScale" priority="25">
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -14639,7 +14981,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="H26:H32">
-    <cfRule type="dataBar" priority="13">
+    <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -14653,40 +14995,50 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="D26:D32">
-    <cfRule type="top10" dxfId="51" priority="12" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="11" priority="13" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="D26:D32">
-    <cfRule type="top10" dxfId="50" priority="11" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="10" priority="12" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="E26:E32">
-    <cfRule type="top10" dxfId="49" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="9" priority="11" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="E26:E32">
-    <cfRule type="top10" dxfId="48" priority="9" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="8" priority="10" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="D26:D32">
-    <cfRule type="top10" dxfId="47" priority="8" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="7" priority="9" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="E26:E32">
-    <cfRule type="top10" dxfId="46" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="6" priority="8" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="F26:F32">
-    <cfRule type="top10" dxfId="45" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="5" priority="7" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="F26:F32">
-    <cfRule type="top10" dxfId="44" priority="5" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="4" priority="6" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="G26:G32">
-    <cfRule type="top10" dxfId="43" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="3" priority="5" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="G26:G32">
-    <cfRule type="top10" dxfId="42" priority="3" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="2" priority="4" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="C26:C32">
-    <cfRule type="top10" dxfId="41" priority="2" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="1" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="C26:C32">
-    <cfRule type="top10" dxfId="40" priority="1" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="0" priority="2" percent="1" bottom="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="C33:G33">
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="4Arrows">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="25"/>
+        <cfvo type="percent" val="50"/>
+        <cfvo type="percent" val="75"/>
+      </iconSet>
+    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId3"/>
@@ -14720,7 +15072,7 @@
           <xm:sqref>H26:H32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" pivot="1">
-          <x14:cfRule type="iconSet" priority="24" id="{15745E97-9939-4517-8A04-29D4F9D687C5}">
+          <x14:cfRule type="iconSet" priority="25" id="{15745E97-9939-4517-8A04-29D4F9D687C5}">
             <x14:iconSet iconSet="3Stars">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -14736,7 +15088,7 @@
           <xm:sqref>C5:C14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" pivot="1">
-          <x14:cfRule type="iconSet" priority="23" id="{04114CB4-E864-4CD6-BA10-54494549D5F4}">
+          <x14:cfRule type="iconSet" priority="24" id="{04114CB4-E864-4CD6-BA10-54494549D5F4}">
             <x14:iconSet iconSet="3Stars">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -14752,7 +15104,7 @@
           <xm:sqref>D5:D14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" pivot="1">
-          <x14:cfRule type="iconSet" priority="22" id="{16DD4843-82D4-4567-86B3-F15723CB8520}">
+          <x14:cfRule type="iconSet" priority="23" id="{16DD4843-82D4-4567-86B3-F15723CB8520}">
             <x14:iconSet iconSet="3Stars">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -14768,7 +15120,7 @@
           <xm:sqref>E5:E14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" pivot="1">
-          <x14:cfRule type="iconSet" priority="21" id="{1D7458E5-6B23-4A90-A3E6-1C9739B17A2D}">
+          <x14:cfRule type="iconSet" priority="22" id="{1D7458E5-6B23-4A90-A3E6-1C9739B17A2D}">
             <x14:iconSet iconSet="3Stars">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -14784,7 +15136,7 @@
           <xm:sqref>F5:F14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" pivot="1">
-          <x14:cfRule type="iconSet" priority="20" id="{B63F468B-07FD-4255-908B-DD90BC519718}">
+          <x14:cfRule type="iconSet" priority="21" id="{B63F468B-07FD-4255-908B-DD90BC519718}">
             <x14:iconSet iconSet="3Stars">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -14803,19 +15155,19 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" high="1" low="1" xr2:uid="{1CF6F669-2EBC-4810-8AE3-F27377EC7C36}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" high="1" low="1" xr2:uid="{E89A34F7-DB47-4450-B6CD-C17BF777A42E}">
+          <x14:colorSeries theme="5"/>
+          <x14:colorNegative theme="6"/>
           <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
+          <x14:colorMarkers theme="5" tint="-0.249977111117893"/>
+          <x14:colorFirst theme="5" tint="-0.249977111117893"/>
+          <x14:colorLast theme="5" tint="-0.249977111117893"/>
+          <x14:colorHigh theme="5" tint="-0.249977111117893"/>
+          <x14:colorLow theme="5" tint="-0.249977111117893"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Expense-Rental'!H5:H14</xm:f>
-              <xm:sqref>H15</xm:sqref>
+              <xm:f>'Expense-Rental'!P4:P111</xm:f>
+              <xm:sqref>P112</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -14855,19 +15207,19 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" high="1" low="1" xr2:uid="{E89A34F7-DB47-4450-B6CD-C17BF777A42E}">
-          <x14:colorSeries theme="5"/>
-          <x14:colorNegative theme="6"/>
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" high="1" low="1" xr2:uid="{1CF6F669-2EBC-4810-8AE3-F27377EC7C36}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers theme="5" tint="-0.249977111117893"/>
-          <x14:colorFirst theme="5" tint="-0.249977111117893"/>
-          <x14:colorLast theme="5" tint="-0.249977111117893"/>
-          <x14:colorHigh theme="5" tint="-0.249977111117893"/>
-          <x14:colorLow theme="5" tint="-0.249977111117893"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Expense-Rental'!P4:P111</xm:f>
-              <xm:sqref>P112</xm:sqref>
+              <xm:f>'Expense-Rental'!H5:H14</xm:f>
+              <xm:sqref>H15</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -14881,7 +15233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93263BDF-1496-4A52-9C4A-10BE87CFB5D0}">
   <dimension ref="B3:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>

</xml_diff>